<commit_message>
Convert different movie formats to image sequence. Images can be saved in grayscale or RGB.
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375"/>
+    <workbookView windowWidth="28800" windowHeight="12375" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="imageSequenceTomovie" sheetId="1" r:id="rId1"/>
+    <sheet name="movieToimageSequence" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Directory where the input image sequence is located.</t>
   </si>
@@ -34,7 +35,7 @@
     <t>Output file extension</t>
   </si>
   <si>
-    <t>Quality</t>
+    <t>Quality (Integer value between 1-10. 1 means lowest quality but maximum compression, 10 means best quality but minimum compression.)</t>
   </si>
   <si>
     <t>Generate all compressions flag</t>
@@ -62,6 +63,24 @@
   </si>
   <si>
     <t>/scratch/utkur/utkarsh/TEMP/SupportingMovieS2_NR_50e_Movie1</t>
+  </si>
+  <si>
+    <t>Input movie which needs to be converted to frames</t>
+  </si>
+  <si>
+    <t>Name of the output directory. Location of the directory where images will be saved. If no value is enetered, a new directory with the name of the video will be created and images saved in that directory.</t>
+  </si>
+  <si>
+    <t>Convertion to grayscale flag. If you want to convert the image sequence to grayscale set it to 1. Default is 0.</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/testVideos/A3 A-road Traffic UK HD - rush hour - British Highway traffic May 2017.mp4</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/testVideos/HTC Sensation FULL HD 1080p Video Sample (highway traffic).mp4</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/testVideos/Relaxing highway traffic_test.mp4</t>
   </si>
 </sst>
 </file>
@@ -69,10 +88,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -91,23 +110,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -121,6 +126,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -134,52 +161,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -192,6 +173,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -199,29 +210,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -234,6 +223,36 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -244,109 +263,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -358,78 +443,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -438,40 +457,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -486,11 +481,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -525,36 +550,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -579,121 +574,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -702,43 +697,46 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1064,152 +1062,220 @@
   <sheetPr/>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="61" customWidth="1"/>
-    <col min="2" max="2" width="10.125" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="12.875" customWidth="1"/>
-    <col min="5" max="5" width="15.125" customWidth="1"/>
-    <col min="6" max="6" width="18.875" customWidth="1"/>
+    <col min="1" max="1" width="61" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="79" customHeight="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="186" customHeight="1" spans="1:8">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>6601</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>5210</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>601</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>811</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>1227</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>1140</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="100.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="85.5" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add parameter for fixing the length of movie.
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="imageSequenceTomovie" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Directory where the input image sequence is located.</t>
   </si>
@@ -27,7 +27,7 @@
     <t>Last frame</t>
   </si>
   <si>
-    <t>File extension</t>
+    <t>Image file extension</t>
   </si>
   <si>
     <t>Output file name. (If no name with path is enetered here '_quality_x.mov' will be added to the input directory name and a movie with that name will be saved. x represents the quality.)</t>
@@ -45,7 +45,7 @@
     <t>Duration of the movie (in seconds. Default value is 20 s.)</t>
   </si>
   <si>
-    <t>/scratch/utkur/utkarsh/TEMP/jp6b07983_si_006</t>
+    <t>/scratch/utkur/utkarsh/TEMP/nl8b04962_si_008</t>
   </si>
   <si>
     <t>.png</t>
@@ -54,19 +54,10 @@
     <t>.mov</t>
   </si>
   <si>
-    <t>/scratch/utkur/utkarsh/TEMP/jp6b07983_si_002</t>
-  </si>
-  <si>
-    <t>/scratch/utkur/utkarsh/TEMP/nl8b04962_si_008</t>
-  </si>
-  <si>
     <t>/scratch/utkur/utkarsh/TEMP/nl500766j_si_002</t>
   </si>
   <si>
     <t>/scratch/utkur/utkarsh/TEMP/nl500766j_si_003</t>
-  </si>
-  <si>
-    <t>/scratch/utkur/utkarsh/TEMP/SupportingMovieS2_NR_50e_Movie1</t>
   </si>
   <si>
     <t>Input movie which needs to be converted to frames</t>
@@ -1156,15 +1147,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3"/>
   <cols>
     <col min="1" max="1" width="61" style="5" customWidth="1"/>
     <col min="2" max="2" width="13.625" style="5" customWidth="1"/>
@@ -1206,7 +1197,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -1214,19 +1205,21 @@
         <v>1</v>
       </c>
       <c r="C2" s="5">
-        <v>6601</v>
+        <v>601</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="E2" s="8"/>
       <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="5">
-        <v>5</v>
+      <c r="G2"/>
+      <c r="H2" s="5">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
@@ -1234,19 +1227,24 @@
         <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>5210</v>
+        <v>811</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="E3" s="8"/>
       <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="5">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8">
+        <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -1254,70 +1252,21 @@
         <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>601</v>
+        <v>1227</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="E4" s="8"/>
       <c r="F4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5">
-        <v>811</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="5">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1227</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1140</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>11</v>
+      <c r="G4" s="5">
+        <v>4</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4" s="8">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1344,18 +1293,18 @@
   <sheetData>
     <row r="1" ht="85.5" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -1363,7 +1312,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5">
         <v>0</v>
@@ -1371,7 +1320,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
@@ -1388,7 +1337,7 @@
   <sheetPr/>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1402,71 +1351,71 @@
   <sheetData>
     <row r="1" ht="25.5" spans="1:10">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" ht="89.25" spans="1:10">
       <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>

</xml_diff>

<commit_message>
Change the default saving movie format to mp4 for better compatibility with windows.
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375"/>
+    <workbookView windowWidth="28800" windowHeight="12105"/>
   </bookViews>
   <sheets>
     <sheet name="imageSequenceTomovie" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Directory where the input image sequence is located.</t>
   </si>
@@ -27,13 +27,13 @@
     <t>Last frame</t>
   </si>
   <si>
-    <t>Image file extension</t>
-  </si>
-  <si>
-    <t>Output file name. (If no name with path is enetered here '_quality_x.mov' will be added to the input directory name and a movie with that name will be saved. x represents the quality.)</t>
-  </si>
-  <si>
-    <t>Output file extension. (Default is .mov file format.)</t>
+    <t>Image file extension. (Default value is '.png')</t>
+  </si>
+  <si>
+    <t>Output file name. (If no name with path is enetered here '_quality_x.mp4' will be added to the input directory name and a movie with that name will be saved. x represents the quality.)</t>
+  </si>
+  <si>
+    <t>Output file extension. (Default is .mp4 file format.)</t>
   </si>
   <si>
     <t>Quality (Integer value between 1-10. 1 means lowest quality but maximum compression, 10 means best quality but minimum compression. Default value is 5.)</t>
@@ -48,16 +48,10 @@
     <t>/scratch/utkur/utkarsh/TEMP/nl8b04962_si_008</t>
   </si>
   <si>
-    <t>.png</t>
-  </si>
-  <si>
-    <t>.mov</t>
+    <t>.avi</t>
   </si>
   <si>
     <t>/scratch/utkur/utkarsh/TEMP/nl500766j_si_002</t>
-  </si>
-  <si>
-    <t>/scratch/utkur/utkarsh/TEMP/nl500766j_si_003</t>
   </si>
   <si>
     <t>Input movie which needs to be converted to frames</t>
@@ -146,10 +140,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -179,23 +173,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,6 +197,104 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -217,47 +303,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,59 +312,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -338,43 +332,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -386,139 +500,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,11 +541,44 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -586,6 +613,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -600,201 +638,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -819,13 +813,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1152,7 +1140,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3"/>
@@ -1165,26 +1153,26 @@
     <col min="6" max="6" width="18.875" style="5" customWidth="1"/>
     <col min="7" max="7" width="15.375" style="5" customWidth="1"/>
     <col min="8" max="8" width="16.75" style="5" customWidth="1"/>
-    <col min="9" max="9" width="17.25" style="8" customWidth="1"/>
+    <col min="9" max="9" width="17.25" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="186" customHeight="1" spans="1:9">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -1193,7 +1181,7 @@
       <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1207,21 +1195,18 @@
       <c r="C2" s="5">
         <v>601</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" s="8"/>
       <c r="F2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2"/>
       <c r="H2" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -1229,45 +1214,15 @@
       <c r="C3" s="5">
         <v>811</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="5">
-        <v>5</v>
-      </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8">
-        <v>50</v>
+      <c r="H3" s="5">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1227</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="5">
-        <v>4</v>
-      </c>
+    <row r="4" spans="8:8">
       <c r="H4"/>
-      <c r="I4" s="8">
-        <v>100</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1293,18 +1248,18 @@
   <sheetData>
     <row r="1" ht="85.5" spans="1:3">
       <c r="A1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -1312,7 +1267,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" s="5">
         <v>0</v>
@@ -1320,7 +1275,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
@@ -1351,71 +1306,71 @@
   <sheetData>
     <row r="1" ht="25.5" spans="1:10">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" ht="89.25" spans="1:10">
       <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>

</xml_diff>

<commit_message>
MPI code to convert seq files to images with global contrast and numpy arrays.
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375" firstSheet="1" activeTab="5"/>
+    <workbookView windowWidth="28800" windowHeight="12375" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="imageSequenceTomovie" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Directory where the input image sequence is located.</t>
   </si>
@@ -132,28 +132,10 @@
     <t>/scratch/utkur/utkarsh/HeatingHolder/Pd-NP/20190523/16-46-00.794.seq</t>
   </si>
   <si>
-    <t>/scratch/utkur/utkarsh/HeatingHolder/Pd-NP/20190523/17-40-29.754.seq</t>
-  </si>
-  <si>
-    <t>/scratch/utkur/utkarsh/HeatingHolder/Pd-NP/20190523/17-51-49.888.seq</t>
-  </si>
-  <si>
     <t>Output directory name. (If no name with path is enetered here a new directory '_process' will be created at the location of input directory and the images will be saved inside the 'crop' folder inside this directory)</t>
   </si>
   <si>
-    <t>/scratch/utkur/utkarsh/HeatingHolder/Pd-NP/20190523/17-40-29.754_Export</t>
-  </si>
-  <si>
-    <t>/scratch/utkur/utkarsh/HeatingHolder/Pd-NP/20190523/17-55-18.290_Export</t>
-  </si>
-  <si>
-    <t>/scratch/utkur/utkarsh/HeatingHolder/Pd-NP/20190523/17-58-26.532_Export</t>
-  </si>
-  <si>
-    <t>/scratch/utkur/utkarsh/HeatingHolder/Pd-NP/20190523/17-58-26.532_Export_avg</t>
-  </si>
-  <si>
-    <t>/scratch/utkur/utkarsh/HeatingHolder/Pd-NP/20190523/18-14-13.112_Export</t>
+    <t>/scratch/utkur/utkarsh/HeatingHolder/Al-Film/05nm/20190718/20190718_16-12-48.635_converted/png</t>
   </si>
 </sst>
 </file>
@@ -815,9 +797,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -1178,79 +1163,79 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="1" width="61" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.75" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.75" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.75" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="61" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.75" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15.375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.75" style="2" customWidth="1"/>
+    <col min="9" max="9" width="17.25" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="186" customHeight="1" spans="1:9">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>601</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G2"/>
-      <c r="H2" s="1">
+      <c r="H2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>811</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1276,43 +1261,43 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="100.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="100.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="42.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="85.5" spans="1:3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1333,69 +1318,69 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="46.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" style="1" customWidth="1"/>
-    <col min="4" max="7" width="15.375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.375" style="4" customWidth="1"/>
-    <col min="9" max="10" width="15.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="46.75" style="2" customWidth="1"/>
+    <col min="2" max="2" width="38.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="2" customWidth="1"/>
+    <col min="4" max="7" width="15.375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.375" style="5" customWidth="1"/>
+    <col min="9" max="10" width="15.375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="114.75" spans="1:10">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7">
         <v>1</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="5:10">
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1408,432 +1393,406 @@
   <sheetPr/>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="57.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.375" style="4" customWidth="1"/>
-    <col min="7" max="8" width="13.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="57.75" style="2" customWidth="1"/>
+    <col min="2" max="2" width="37.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.375" style="5" customWidth="1"/>
+    <col min="7" max="8" width="13.125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="114.75" spans="1:8">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7">
         <v>0.5</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="6">
-        <v>1</v>
-      </c>
-      <c r="H2" s="6">
-        <v>100</v>
+      <c r="F2" s="9"/>
+      <c r="G2" s="7">
+        <v>400</v>
+      </c>
+      <c r="H2" s="7">
+        <v>550</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="6">
-        <v>300</v>
-      </c>
-      <c r="H3" s="6">
-        <v>350</v>
-      </c>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="6">
-        <v>50</v>
-      </c>
-      <c r="H4" s="6">
-        <v>150</v>
-      </c>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1854,50 +1813,50 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="61" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.75" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.75" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="61" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.75" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="99.75" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>39</v>
+      <c r="E1" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>601</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>811</v>
       </c>
     </row>
@@ -1910,89 +1869,45 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="73.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.75" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="79.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.75" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="186" customHeight="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="57" spans="1:4">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" ht="28.5" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="1">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <v>207642</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>53108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>136908</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>136908</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>345328</v>
+      <c r="C2" s="2">
+        <v>11899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Find the coordinates of cropped image from the original image using template matching.
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375" firstSheet="1" activeTab="3"/>
+    <workbookView windowWidth="28800" windowHeight="12375" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="imageSequenceTomovie" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="convertSeqFiles" sheetId="4" r:id="rId4"/>
     <sheet name="cropImageSequence" sheetId="6" r:id="rId5"/>
     <sheet name="deleteImageSequence" sheetId="7" r:id="rId6"/>
+    <sheet name="findCropInImage" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>Directory where the input image sequence is located.</t>
   </si>
@@ -136,6 +137,33 @@
   </si>
   <si>
     <t>/scratch/utkur/utkarsh/HeatingHolder/Al-Film/05nm/20190718/20190718_16-12-48.635_converted/png</t>
+  </si>
+  <si>
+    <t>Crop image file name with location</t>
+  </si>
+  <si>
+    <t>Original image from where the image was cropped.</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/000401-1.png</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/000401.png</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/000401-2.png</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/000401-3.png</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/000401-4.png</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/000401-5.png</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/000401-6.png</t>
   </si>
 </sst>
 </file>
@@ -184,8 +212,106 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -206,14 +332,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -223,102 +341,12 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -347,19 +375,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -371,25 +537,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,127 +549,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -599,16 +627,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -634,16 +662,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -652,152 +680,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -808,9 +836,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
@@ -1213,7 +1238,7 @@
       <c r="C2" s="2">
         <v>601</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="1"/>
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1267,7 +1292,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="85.5" spans="1:3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1322,65 +1347,65 @@
     <col min="2" max="2" width="38.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="22.5" style="2" customWidth="1"/>
     <col min="4" max="7" width="15.375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="15.375" style="4" customWidth="1"/>
     <col min="9" max="10" width="15.375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="114.75" spans="1:10">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6">
         <v>1</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="5:10">
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1393,7 +1418,7 @@
   <sheetPr/>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
@@ -1406,393 +1431,393 @@
     <col min="3" max="3" width="16.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.375" style="2" customWidth="1"/>
     <col min="5" max="5" width="20.625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.375" style="4" customWidth="1"/>
     <col min="7" max="8" width="13.125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="114.75" spans="1:8">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6">
         <v>0.5</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="7">
+      <c r="F2" s="8"/>
+      <c r="G2" s="6">
         <v>400</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="6">
         <v>550</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1847,7 +1872,7 @@
       <c r="C2" s="2">
         <v>601</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
@@ -1914,4 +1939,83 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="60" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Archive a directory for easy transfer to dropbox or any other backup server.
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375" tabRatio="779"/>
+    <workbookView windowWidth="28800" windowHeight="12375" tabRatio="779" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="imageSequenceTomovie" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="deleteImageSequence" sheetId="7" r:id="rId6"/>
     <sheet name="findCropInImage" sheetId="9" r:id="rId7"/>
     <sheet name="movingAverageImages" sheetId="10" r:id="rId8"/>
+    <sheet name="archiveFolder" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
   <si>
     <t>Directory where the input image sequence is located.</t>
   </si>
@@ -212,10 +213,19 @@
     <t>Normalize Flag (Set to 1 if you want to normalize the image. Otherwise set to 0. Default is 0.)</t>
   </si>
   <si>
-    <t>/home/utkarsh/Desktop/restorePillars/LC1/01_HM_badchip_wet_converted/output/driftCorrectNPY</t>
-  </si>
-  <si>
-    <t>npy</t>
+    <t>/home/utkarsh/Desktop/restorePillars/LC1/01_HM_badchip_wet_converted/output/driftCorrectPNG</t>
+  </si>
+  <si>
+    <t>png</t>
+  </si>
+  <si>
+    <t>Delete flag (Set to 1 if you want to delete the directory after archiving. 0 otherwise. Default is 0)</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/exSitu</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/StarTracker</t>
   </si>
 </sst>
 </file>
@@ -224,9 +234,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -270,6 +280,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -285,22 +302,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -316,10 +319,26 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -339,30 +358,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -377,30 +403,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -427,55 +437,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,127 +605,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -676,6 +686,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -690,17 +715,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -722,158 +743,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -899,10 +909,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1265,7 +1275,7 @@
   <sheetPr/>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1539,7 +1549,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>
@@ -1585,7 +1595,7 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="16"/>
@@ -1595,21 +1605,21 @@
       <c r="D2" s="16">
         <v>1</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="6">
         <v>1</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="6">
         <v>0.1</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="6">
         <v>99.9</v>
       </c>
       <c r="H2" s="18"/>
-      <c r="I2" s="5">
+      <c r="I2" s="6">
         <v>55967</v>
       </c>
-      <c r="J2" s="5">
-        <v>59101</v>
+      <c r="J2" s="6">
+        <v>66634</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1617,12 +1627,12 @@
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="18"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1679,362 +1689,362 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6">
         <v>0.5</v>
       </c>
       <c r="F2" s="13"/>
-      <c r="G2" s="5">
+      <c r="G2" s="6">
         <v>400</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="6">
         <v>550</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
       <c r="F3" s="13"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="13"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="13"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
       <c r="F17" s="13"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
       <c r="F18" s="13"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
       <c r="F19" s="13"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
       <c r="F20" s="13"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
       <c r="F21" s="13"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
       <c r="F22" s="13"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
       <c r="F23" s="13"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
       <c r="F24" s="13"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
       <c r="F25" s="13"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
       <c r="F26" s="13"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
       <c r="F27" s="13"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
       <c r="F28" s="13"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
       <c r="F29" s="13"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
       <c r="F30" s="13"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
       <c r="F31" s="13"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
       <c r="F32" s="13"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
       <c r="F33" s="13"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
       <c r="F34" s="13"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
       <c r="F35" s="13"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
       <c r="F36" s="13"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
       <c r="F37" s="13"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2166,7 +2176,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -2220,7 +2230,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3"/>
@@ -2260,57 +2270,112 @@
       <c r="H1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" ht="25.5" spans="1:10">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5">
-        <v>3126</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6">
+        <v>55967</v>
+      </c>
+      <c r="D2" s="6">
+        <v>66625</v>
+      </c>
+      <c r="E2" s="6">
         <v>30</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="6">
         <v>0</v>
       </c>
-      <c r="H2" s="5">
-        <v>1</v>
+      <c r="H2" s="6">
+        <v>0</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="50.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.25" style="1" customWidth="1"/>
+    <col min="3" max="4" width="15.375" style="2" customWidth="1"/>
+    <col min="5" max="16378" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="63.75" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Use 7z command line arguments to zip the files. Faster and better compression.
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
   <si>
     <t>Directory where the input image sequence is located.</t>
   </si>
@@ -219,6 +219,9 @@
     <t>png</t>
   </si>
   <si>
+    <t>Directory which you want to archive</t>
+  </si>
+  <si>
     <t>Delete flag (Set to 1 if you want to delete the directory after archiving. 0 otherwise. Default is 0)</t>
   </si>
   <si>
@@ -226,6 +229,9 @@
   </si>
   <si>
     <t>/home/utkarsh/Desktop/StarTracker</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/Test/png_avg</t>
   </si>
 </sst>
 </file>
@@ -234,9 +240,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -281,7 +287,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -296,7 +302,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -310,9 +316,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -326,9 +362,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -336,22 +371,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -372,16 +392,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -394,11 +407,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -408,13 +421,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -437,25 +443,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,157 +623,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -670,6 +676,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -681,21 +696,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -726,6 +726,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -734,146 +749,137 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -883,7 +889,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2331,15 +2337,15 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="50.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.25" style="1" customWidth="1"/>
@@ -2349,10 +2355,10 @@
   <sheetData>
     <row r="1" ht="63.75" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -2360,7 +2366,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
@@ -2368,14 +2374,151 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="2:2">
-      <c r="B4" s="6"/>
+    <row r="4" spans="1:2">
+      <c r="A4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Helper function for reading all the split files.
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375" tabRatio="779" firstSheet="2" activeTab="8"/>
+    <workbookView windowWidth="28800" windowHeight="12375" tabRatio="779" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="imageSequenceTomovie" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,15 @@
     <sheet name="findCropInImage" sheetId="9" r:id="rId7"/>
     <sheet name="movingAverageImages" sheetId="10" r:id="rId8"/>
     <sheet name="archiveFolder" sheetId="11" r:id="rId9"/>
+    <sheet name="splitFiles" sheetId="12" r:id="rId10"/>
+    <sheet name="joinFiles" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
   <si>
     <t>Directory where the input image sequence is located.</t>
   </si>
@@ -225,13 +227,19 @@
     <t>Delete flag (Set to 1 if you want to delete the directory after archiving. 0 otherwise. Default is 0)</t>
   </si>
   <si>
-    <t>/home/utkarsh/Desktop/exSitu</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/StarTracker</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/Test/png_avg</t>
+    <t>/home/utkarsh/Desktop/restorePillars/LC2/01_HM_badChip_wet_bulk_converted</t>
+  </si>
+  <si>
+    <t>File with path which you want to split</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Projects/Datasets/Vehicles/Seattle Traffic in 5K 360° VR Video - Seattle Highways &amp; Stadiums.webm</t>
+  </si>
+  <si>
+    <t>File with path which you want to join</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/restorePillars/LC2/01_HM_badChip_wet_bulk_converted.zip_split_0001</t>
   </si>
 </sst>
 </file>
@@ -239,10 +247,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -287,7 +295,60 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -296,13 +357,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -317,29 +371,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -347,18 +378,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -384,17 +408,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -407,16 +422,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -443,97 +451,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,85 +625,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,6 +660,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -663,15 +680,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -715,17 +723,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -749,147 +746,158 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1490,6 +1498,382 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="50.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.25" style="1" customWidth="1"/>
+    <col min="3" max="4" width="15.375" style="2" customWidth="1"/>
+    <col min="5" max="16378" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="63.75" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" ht="25.5" spans="1:4">
+      <c r="A2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="50.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.25" style="1" customWidth="1"/>
+    <col min="3" max="4" width="15.375" style="2" customWidth="1"/>
+    <col min="5" max="16378" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="63.75" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" ht="25.5" spans="1:4">
+      <c r="A2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
@@ -2339,10 +2723,10 @@
   <sheetPr/>
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
@@ -2364,7 +2748,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" ht="25.5" spans="1:4">
       <c r="A2" s="6" t="s">
         <v>67</v>
       </c>
@@ -2373,20 +2757,14 @@
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="6" t="s">
-        <v>68</v>
-      </c>
+      <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="6"/>

</xml_diff>

<commit_message>
Add save option to another directory.
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
   <si>
     <t>Directory where the input image sequence is located.</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>File with path which you want to split</t>
+  </si>
+  <si>
+    <t>Output durectory. Leave blank if you wish to save the split files in-place.</t>
   </si>
   <si>
     <t>/home/utkarsh/Projects/Datasets/Vehicles/Seattle Traffic in 5K 360° VR Video - Seattle Highways &amp; Stadiums.webm</t>
@@ -249,8 +252,8 @@
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -301,16 +304,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -331,13 +334,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -346,27 +342,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -402,14 +381,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -422,6 +409,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,97 +460,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -559,79 +634,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -660,15 +663,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -680,6 +674,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -709,6 +712,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -719,21 +737,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -762,82 +765,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -846,34 +849,34 @@
     <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -882,19 +885,19 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1501,184 +1504,223 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="50.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.25" style="1" customWidth="1"/>
-    <col min="3" max="4" width="15.375" style="2" customWidth="1"/>
-    <col min="5" max="16378" width="9" style="3"/>
+    <col min="1" max="2" width="50.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.25" style="1" customWidth="1"/>
+    <col min="4" max="5" width="15.375" style="2" customWidth="1"/>
+    <col min="6" max="16379" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="63.75" spans="1:5">
+    <row r="1" ht="63.75" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
-    </row>
-    <row r="2" ht="25.5" spans="1:4">
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" ht="25.5" spans="1:5">
       <c r="A2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="6">
+        <v>70</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
       <c r="D2" s="7"/>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1707,7 +1749,7 @@
   <sheetData>
     <row r="1" ht="63.75" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>66</v>
@@ -1718,7 +1760,7 @@
     </row>
     <row r="2" ht="25.5" spans="1:4">
       <c r="A2" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>

</xml_diff>

<commit_message>
Now zip can also be used to archive folders.
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375" tabRatio="779" firstSheet="2" activeTab="9"/>
+    <workbookView windowWidth="28800" windowHeight="12375" tabRatio="779" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="imageSequenceTomovie" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="archiveFolder" sheetId="11" r:id="rId9"/>
     <sheet name="splitFiles" sheetId="12" r:id="rId10"/>
     <sheet name="joinFiles" sheetId="13" r:id="rId11"/>
+    <sheet name="dropboxUpload" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="86">
   <si>
     <t>Directory where the input image sequence is located.</t>
   </si>
@@ -227,7 +228,7 @@
     <t>Delete flag (Set to 1 if you want to delete the directory after archiving. 0 otherwise. Default is 0)</t>
   </si>
   <si>
-    <t>/home/utkarsh/Desktop/restorePillars/LC2/01_HM_badChip_wet_bulk_converted</t>
+    <t>/home/utkarsh/Desktop/restorePillars/LC1</t>
   </si>
   <si>
     <t>File with path which you want to split</t>
@@ -243,6 +244,45 @@
   </si>
   <si>
     <t>/home/utkarsh/Desktop/restorePillars/LC2/01_HM_badChip_wet_bulk_converted.zip_split_0001</t>
+  </si>
+  <si>
+    <t>File which you want to upload on Dropbox</t>
+  </si>
+  <si>
+    <t>Folder where you want to upload it on Dropbox</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Projects/Datasets/Vehicles/Seattle Traffic in 5K 360° VR Video - Seattle Highways &amp; Stadiums.webm_split_0008</t>
+  </si>
+  <si>
+    <t>/Utkarsh</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/Photos.zip</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Projects/Datasets/Vehicles/HTC Sensation FULL HD 1080p Video Sample (highway traffic).mp4</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Projects/Datasets/Vehicles/A3 A-road Traffic UK HD - rush hour - British Highway traffic May 2017.mp4</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Projects/Datasets/Vehicles/Relaxing highway traffic.webm</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Projects/Datasets/Vehicles/M6 Motorway Traffic.mp4</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Projects/Datasets/Vehicles/non-vehicles.zip</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Projects/Datasets/Vehicles/vehicles.zip</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Projects/Datasets/Vehicles/Driving in Singapore 4k.mp4</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Projects/Datasets/Vehicles/Seattle Traffic in 5K 360° VR Video - Seattle Highways &amp; Stadiums.webm_split_0007</t>
   </si>
 </sst>
 </file>
@@ -251,9 +291,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -304,16 +344,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -357,14 +405,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -380,10 +420,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -394,16 +451,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -417,17 +466,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -466,7 +506,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,60 +656,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -544,97 +668,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -687,15 +727,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -707,21 +738,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -743,15 +759,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -760,144 +767,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1506,7 +1546,7 @@
   <sheetPr/>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1808,6 +1848,228 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="2" width="50.375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="15.375" style="2" customWidth="1"/>
+    <col min="5" max="16378" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" ht="25.5" spans="1:4">
+      <c r="A2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" ht="25.5" spans="1:2">
+      <c r="A4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" ht="25.5" spans="1:2">
+      <c r="A5" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" ht="25.5" spans="1:2">
+      <c r="A6" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" ht="25.5" spans="1:2">
+      <c r="A10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" ht="25.5" spans="1:2">
+      <c r="A11" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
       <c r="B12" s="6"/>
     </row>
     <row r="13" spans="1:2">
@@ -2790,7 +3052,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" ht="25.5" spans="1:4">
+    <row r="2" spans="1:4">
       <c r="A2" s="6" t="s">
         <v>67</v>
       </c>

</xml_diff>

<commit_message>
Upload files to Dropbox using API v2.
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="79">
   <si>
     <t>Directory where the input image sequence is located.</t>
   </si>
@@ -228,7 +228,7 @@
     <t>Delete flag (Set to 1 if you want to delete the directory after archiving. 0 otherwise. Default is 0)</t>
   </si>
   <si>
-    <t>/home/utkarsh/Desktop/restorePillars/LC1</t>
+    <t>/home/utkarsh/Desktop/restorePillars/LC2/01_HM_badChip_wet_bulk_converted/npy</t>
   </si>
   <si>
     <t>File with path which you want to split</t>
@@ -252,37 +252,16 @@
     <t>Folder where you want to upload it on Dropbox</t>
   </si>
   <si>
-    <t>/home/utkarsh/Projects/Datasets/Vehicles/Seattle Traffic in 5K 360° VR Video - Seattle Highways &amp; Stadiums.webm_split_0008</t>
-  </si>
-  <si>
-    <t>/Utkarsh</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/Photos.zip</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Projects/Datasets/Vehicles/HTC Sensation FULL HD 1080p Video Sample (highway traffic).mp4</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Projects/Datasets/Vehicles/A3 A-road Traffic UK HD - rush hour - British Highway traffic May 2017.mp4</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Projects/Datasets/Vehicles/Relaxing highway traffic.webm</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Projects/Datasets/Vehicles/M6 Motorway Traffic.mp4</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Projects/Datasets/Vehicles/non-vehicles.zip</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Projects/Datasets/Vehicles/vehicles.zip</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Projects/Datasets/Vehicles/Driving in Singapore 4k.mp4</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Projects/Datasets/Vehicles/Seattle Traffic in 5K 360° VR Video - Seattle Highways &amp; Stadiums.webm_split_0007</t>
+    <t>/home/utkarsh/Desktop/DropboxUploadTest/MNIST/emnist-bymerge.mat</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/DropboxUploadTest/MNIST/emnist-digits.mat</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/DropboxUploadTest/MNIST/emnist-letters.mat</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Desktop/DropboxUploadTest/MNIST/emnist-mnist.mat</t>
   </si>
 </sst>
 </file>
@@ -290,10 +269,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -304,12 +283,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="1"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="1"/>
@@ -337,8 +316,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -352,38 +346,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -399,6 +371,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -412,9 +392,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -428,9 +407,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -444,23 +422,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -494,187 +473,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -727,6 +706,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -738,6 +741,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -759,41 +773,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -805,130 +784,130 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -937,10 +916,10 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -954,27 +933,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -987,10 +966,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
@@ -1005,7 +984,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
@@ -1554,8 +1533,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="2" width="50.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.25" style="1" customWidth="1"/>
+    <col min="1" max="2" width="50.375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.25" style="6" customWidth="1"/>
     <col min="4" max="5" width="15.375" style="2" customWidth="1"/>
     <col min="6" max="16379" width="9" style="3"/>
   </cols>
@@ -1575,192 +1554,192 @@
       <c r="F1" s="5"/>
     </row>
     <row r="2" ht="25.5" spans="1:5">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1">
         <v>0</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1781,8 +1760,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="50.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="18.25" style="6" customWidth="1"/>
     <col min="3" max="4" width="15.375" style="2" customWidth="1"/>
     <col min="5" max="16378" width="9" style="3"/>
   </cols>
@@ -1799,156 +1778,156 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" ht="25.5" spans="1:4">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1959,7 +1938,7 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1967,7 +1946,7 @@
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="2" width="50.375" style="1" customWidth="1"/>
     <col min="3" max="4" width="15.375" style="2" customWidth="1"/>
@@ -1985,192 +1964,25 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" ht="25.5" spans="1:4">
-      <c r="A2" s="6" t="s">
+    <row r="2" ht="25.5" spans="1:1">
+      <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="6" t="s">
+    </row>
+    <row r="3" ht="25.5" spans="1:1">
+      <c r="A3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="6" t="s">
+    </row>
+    <row r="4" ht="25.5" spans="1:1">
+      <c r="A4" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" ht="25.5" spans="1:2">
-      <c r="A4" s="6" t="s">
+    </row>
+    <row r="5" ht="25.5" spans="1:1">
+      <c r="A5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" ht="25.5" spans="1:2">
-      <c r="A5" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" ht="25.5" spans="1:2">
-      <c r="A6" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" ht="25.5" spans="1:2">
-      <c r="A10" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" ht="25.5" spans="1:2">
-      <c r="A11" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2">
-      <c r="B12" s="6"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2289,7 +2101,7 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="16"/>
@@ -2299,20 +2111,20 @@
       <c r="D2" s="16">
         <v>1</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="1">
         <v>0.1</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="1">
         <v>99.9</v>
       </c>
       <c r="H2" s="18"/>
-      <c r="I2" s="6">
+      <c r="I2" s="1">
         <v>55967</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="1">
         <v>66634</v>
       </c>
     </row>
@@ -2321,12 +2133,12 @@
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
       <c r="H3" s="18"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2383,362 +2195,362 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1">
         <v>0.5</v>
       </c>
       <c r="F2" s="13"/>
-      <c r="G2" s="6">
+      <c r="G2" s="1">
         <v>400</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="1">
         <v>550</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
       <c r="F3" s="13"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="13"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
       <c r="F16" s="13"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
       <c r="F17" s="13"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="13"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
       <c r="F19" s="13"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
       <c r="F20" s="13"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
       <c r="F21" s="13"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
       <c r="F22" s="13"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
       <c r="F23" s="13"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
       <c r="F24" s="13"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
       <c r="F25" s="13"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
       <c r="F26" s="13"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
       <c r="F27" s="13"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
       <c r="F28" s="13"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
       <c r="F29" s="13"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
       <c r="F30" s="13"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
       <c r="F31" s="13"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
       <c r="F32" s="13"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
       <c r="F33" s="13"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
       <c r="F34" s="13"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
       <c r="F35" s="13"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
       <c r="F36" s="13"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
       <c r="F37" s="13"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2929,12 +2741,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="1" width="50.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" style="1" customWidth="1"/>
-    <col min="4" max="6" width="15.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="38.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="6" customWidth="1"/>
+    <col min="4" max="6" width="15.375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="18.25" style="6" customWidth="1"/>
+    <col min="8" max="8" width="15.375" style="6" customWidth="1"/>
     <col min="9" max="10" width="15.375" style="2" customWidth="1"/>
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
@@ -2969,52 +2781,52 @@
       <c r="K1" s="5"/>
     </row>
     <row r="2" ht="25.5" spans="1:10">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1">
         <v>55967</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="1">
         <v>66625</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="1">
         <v>30</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="1">
         <v>0</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3030,13 +2842,13 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="50.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="18.25" style="6" customWidth="1"/>
     <col min="3" max="4" width="15.375" style="2" customWidth="1"/>
     <col min="5" max="16378" width="9" style="3"/>
   </cols>
@@ -3052,155 +2864,155 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="6" t="s">
+    <row r="2" ht="25.5" spans="1:4">
+      <c r="A2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="1"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>